<commit_message>
Attempting to run wtk fetching for Bergey data
</commit_message>
<xml_diff>
--- a/notebooks/validation/01 One Energy Turbine Data/OneEnergyTurbineData.xlsx
+++ b/notebooks/validation/01 One Energy Turbine Data/OneEnergyTurbineData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruzekow/dw-tap/notebooks/validation/01 One Energy Turbine Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFE49EEF-BF36-F54E-A75B-0E9C85653D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DC86B3-50B5-8349-ABEE-03C7644FF45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="12960" windowHeight="16140" xr2:uid="{2C7B4680-893B-4A42-8DA2-9636C056BE27}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="26100" windowHeight="16100" xr2:uid="{2C7B4680-893B-4A42-8DA2-9636C056BE27}"/>
   </bookViews>
   <sheets>
     <sheet name="Turbines" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
   <si>
     <t>APRS ID</t>
   </si>
@@ -178,6 +178,54 @@
   </si>
   <si>
     <t>p6l3</t>
+  </si>
+  <si>
+    <t>Links to pages on a2e</t>
+  </si>
+  <si>
+    <t>periods with consistent generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add column </t>
+  </si>
+  <si>
+    <t xml:space="preserve">next steps: </t>
+  </si>
+  <si>
+    <t>read into python</t>
+  </si>
+  <si>
+    <t>turn lat lon into goemetry column</t>
+  </si>
+  <si>
+    <t>make into geojson file for QGIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what do these sites look like? </t>
+  </si>
+  <si>
+    <t>what is the obstacle set up looking like?</t>
+  </si>
+  <si>
+    <t>radius of 100m around point</t>
+  </si>
+  <si>
+    <t>radius of 1000m around point</t>
+  </si>
+  <si>
+    <t>column buildings within 100m</t>
+  </si>
+  <si>
+    <t>very simple analysis if no buildings are in the region</t>
+  </si>
+  <si>
+    <t>backup: look at google maps</t>
+  </si>
+  <si>
+    <t>todo: try the get data notebook</t>
+  </si>
+  <si>
+    <t>take notes of what breaks</t>
   </si>
 </sst>
 </file>
@@ -543,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2407F861-3A91-8D4F-B2B3-4B39768EBFAE}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,7 +609,7 @@
     <col min="9" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,22 +623,22 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -604,22 +652,22 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F2">
-        <v>87</v>
+        <v>41.101219</v>
       </c>
       <c r="G2">
-        <v>1500</v>
+        <v>-83.644394000000005</v>
       </c>
       <c r="H2">
-        <v>41.101219</v>
+        <v>80</v>
       </c>
       <c r="I2">
-        <v>-83.644394000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -633,22 +681,22 @@
         <v>7</v>
       </c>
       <c r="E3">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F3">
-        <v>87</v>
+        <v>41.09975</v>
       </c>
       <c r="G3">
-        <v>1500</v>
+        <v>-83.643533000000005</v>
       </c>
       <c r="H3">
-        <v>41.09975</v>
+        <v>80</v>
       </c>
       <c r="I3">
-        <v>-83.643533000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -662,22 +710,22 @@
         <v>7</v>
       </c>
       <c r="E4" s="1">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F4" s="1">
-        <v>87</v>
+        <v>41.097669000000003</v>
       </c>
       <c r="G4" s="1">
-        <v>1500</v>
+        <v>-83.642588000000003</v>
       </c>
       <c r="H4" s="1">
-        <v>41.097669000000003</v>
+        <v>80</v>
       </c>
       <c r="I4" s="1">
-        <v>-83.642588000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -691,22 +739,22 @@
         <v>7</v>
       </c>
       <c r="E5" s="1">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F5" s="1">
-        <v>87</v>
+        <v>41.096111000000001</v>
       </c>
       <c r="G5" s="1">
-        <v>1500</v>
+        <v>-83.641379999999998</v>
       </c>
       <c r="H5" s="1">
-        <v>41.096111000000001</v>
+        <v>80</v>
       </c>
       <c r="I5" s="1">
-        <v>-83.641379999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -720,22 +768,22 @@
         <v>7</v>
       </c>
       <c r="E6" s="1">
-        <v>80</v>
-      </c>
-      <c r="F6" s="1">
-        <v>87</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H6">
+        <v>87</v>
+      </c>
+      <c r="F6">
         <v>41.094388000000002</v>
       </c>
-      <c r="I6">
+      <c r="G6">
         <v>-83.639116000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H6" s="1">
+        <v>80</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -749,22 +797,22 @@
         <v>7</v>
       </c>
       <c r="E7" s="1">
-        <v>80</v>
-      </c>
-      <c r="F7" s="1">
-        <v>87</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H7">
+        <v>87</v>
+      </c>
+      <c r="F7">
         <v>41.093077999999998</v>
       </c>
-      <c r="I7">
+      <c r="G7">
         <v>-83.637777</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H7" s="1">
+        <v>80</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -778,22 +826,22 @@
         <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>80</v>
-      </c>
-      <c r="F8" s="1">
-        <v>87</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H8">
+        <v>87</v>
+      </c>
+      <c r="F8">
         <v>41.091914000000003</v>
       </c>
-      <c r="I8">
+      <c r="G8">
         <v>-83.636667000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H8" s="1">
+        <v>80</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -807,22 +855,22 @@
         <v>7</v>
       </c>
       <c r="E9" s="1">
-        <v>80</v>
-      </c>
-      <c r="F9" s="1">
-        <v>87</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H9">
+        <v>87</v>
+      </c>
+      <c r="F9">
         <v>41.088397999999998</v>
       </c>
-      <c r="I9">
+      <c r="G9">
         <v>-83.636595999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H9" s="1">
+        <v>80</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -836,22 +884,22 @@
         <v>7</v>
       </c>
       <c r="E10" s="1">
-        <v>80</v>
-      </c>
-      <c r="F10" s="1">
-        <v>87</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H10">
+        <v>87</v>
+      </c>
+      <c r="F10">
         <v>41.082611</v>
       </c>
-      <c r="I10">
+      <c r="G10">
         <v>-83.643974999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" s="1">
+        <v>80</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -865,22 +913,23 @@
         <v>7</v>
       </c>
       <c r="E11" s="1">
-        <v>80</v>
-      </c>
-      <c r="F11" s="1">
-        <v>87</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H11">
+        <v>87</v>
+      </c>
+      <c r="F11">
         <v>41.084657999999997</v>
       </c>
-      <c r="I11">
+      <c r="G11">
         <v>-83.644558000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H11" s="1">
+        <v>80</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1500</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -894,22 +943,23 @@
         <v>7</v>
       </c>
       <c r="E12" s="1">
-        <v>80</v>
-      </c>
-      <c r="F12" s="1">
-        <v>87</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H12">
+        <v>87</v>
+      </c>
+      <c r="F12">
         <v>40.127906000000003</v>
       </c>
-      <c r="I12">
+      <c r="G12">
         <v>-84.615171000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H12" s="1">
+        <v>80</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1500</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -923,22 +973,23 @@
         <v>7</v>
       </c>
       <c r="E13" s="1">
-        <v>80</v>
-      </c>
-      <c r="F13" s="1">
-        <v>87</v>
+        <v>87</v>
+      </c>
+      <c r="F13">
+        <v>40.127878000000003</v>
       </c>
       <c r="G13" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H13">
-        <v>40.127878000000003</v>
+        <v>-84.611106000000007</v>
+      </c>
+      <c r="H13" s="1">
+        <v>80</v>
       </c>
       <c r="I13" s="1">
-        <v>-84.611106000000007</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -952,22 +1003,23 @@
         <v>7</v>
       </c>
       <c r="E14" s="1">
-        <v>80</v>
-      </c>
-      <c r="F14" s="1">
-        <v>87</v>
+        <v>87</v>
+      </c>
+      <c r="F14">
+        <v>40.127690000000001</v>
       </c>
       <c r="G14" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H14">
-        <v>40.127690000000001</v>
+        <v>-84.608220000000003</v>
+      </c>
+      <c r="H14" s="1">
+        <v>80</v>
       </c>
       <c r="I14" s="1">
-        <v>-84.608220000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -981,22 +1033,23 @@
         <v>7</v>
       </c>
       <c r="E15" s="1">
-        <v>80</v>
-      </c>
-      <c r="F15" s="1">
-        <v>87</v>
+        <v>87</v>
+      </c>
+      <c r="F15">
+        <v>40.718290000000003</v>
       </c>
       <c r="G15" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H15">
-        <v>40.718290000000003</v>
+        <v>-83.228650000000002</v>
+      </c>
+      <c r="H15" s="1">
+        <v>80</v>
       </c>
       <c r="I15" s="1">
-        <v>-83.228650000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1010,22 +1063,23 @@
         <v>7</v>
       </c>
       <c r="E16" s="1">
-        <v>80</v>
-      </c>
-      <c r="F16" s="1">
-        <v>87</v>
+        <v>87</v>
+      </c>
+      <c r="F16">
+        <v>40.591555</v>
       </c>
       <c r="G16" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H16">
-        <v>40.591555</v>
+        <v>-83.182091999999997</v>
+      </c>
+      <c r="H16" s="1">
+        <v>80</v>
       </c>
       <c r="I16" s="1">
-        <v>-83.182091999999997</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1039,22 +1093,23 @@
         <v>7</v>
       </c>
       <c r="E17" s="1">
-        <v>80</v>
-      </c>
-      <c r="F17" s="1">
-        <v>87</v>
+        <v>87</v>
+      </c>
+      <c r="F17">
+        <v>40.591154000000003</v>
       </c>
       <c r="G17" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H17">
-        <v>40.591154000000003</v>
+        <v>-83.178490999999994</v>
+      </c>
+      <c r="H17" s="1">
+        <v>80</v>
       </c>
       <c r="I17" s="1">
-        <v>-83.178490999999994</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1068,22 +1123,23 @@
         <v>7</v>
       </c>
       <c r="E18" s="1">
-        <v>80</v>
-      </c>
-      <c r="F18" s="1">
-        <v>87</v>
+        <v>87</v>
+      </c>
+      <c r="F18">
+        <v>40.590772999999999</v>
       </c>
       <c r="G18" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H18">
-        <v>40.590772999999999</v>
+        <v>-83.174941000000004</v>
+      </c>
+      <c r="H18" s="1">
+        <v>80</v>
       </c>
       <c r="I18" s="1">
-        <v>-83.174941000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1097,22 +1153,23 @@
         <v>7</v>
       </c>
       <c r="E19" s="1">
-        <v>80</v>
-      </c>
-      <c r="F19" s="1">
-        <v>87</v>
+        <v>87</v>
+      </c>
+      <c r="F19">
+        <v>41.002763999999999</v>
       </c>
       <c r="G19" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H19">
-        <v>41.002763999999999</v>
+        <v>-84.033742000000004</v>
+      </c>
+      <c r="H19" s="1">
+        <v>80</v>
       </c>
       <c r="I19" s="1">
-        <v>-84.033742000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1126,22 +1183,23 @@
         <v>7</v>
       </c>
       <c r="E20" s="1">
-        <v>80</v>
-      </c>
-      <c r="F20" s="1">
-        <v>87</v>
+        <v>87</v>
+      </c>
+      <c r="F20">
+        <v>41.192379000000003</v>
       </c>
       <c r="G20" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H20">
-        <v>41.192379000000003</v>
+        <v>-84.612841000000003</v>
+      </c>
+      <c r="H20" s="1">
+        <v>80</v>
       </c>
       <c r="I20" s="1">
-        <v>-84.612841000000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1155,22 +1213,23 @@
         <v>7</v>
       </c>
       <c r="E21" s="1">
-        <v>80</v>
-      </c>
-      <c r="F21" s="1">
-        <v>87</v>
+        <v>87</v>
+      </c>
+      <c r="F21">
+        <v>41.189914000000002</v>
       </c>
       <c r="G21" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H21">
-        <v>41.189914000000002</v>
+        <v>-84.612858000000003</v>
+      </c>
+      <c r="H21" s="1">
+        <v>80</v>
       </c>
       <c r="I21" s="1">
-        <v>-84.612858000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1184,20 +1243,99 @@
         <v>7</v>
       </c>
       <c r="E22" s="1">
-        <v>80</v>
-      </c>
-      <c r="F22" s="1">
-        <v>87</v>
+        <v>87</v>
+      </c>
+      <c r="F22">
+        <v>41.187455</v>
       </c>
       <c r="G22" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H22">
-        <v>41.187455</v>
+        <v>-84.612875000000003</v>
+      </c>
+      <c r="H22" s="1">
+        <v>80</v>
       </c>
       <c r="I22" s="1">
-        <v>-84.612875000000003</v>
-      </c>
+        <v>1500</v>
+      </c>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E48" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1207,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F386DA0-7548-6E42-81AF-527B6329B36A}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1297,6 +1435,86 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Prepared and combined data for One Energy and some of the original data files
</commit_message>
<xml_diff>
--- a/notebooks/validation/01 One Energy Turbine Data/OneEnergyTurbineData.xlsx
+++ b/notebooks/validation/01 One Energy Turbine Data/OneEnergyTurbineData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruzekow/dw-tap/notebooks/validation/01 One Energy Turbine Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DC86B3-50B5-8349-ABEE-03C7644FF45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5624F1E-D86A-EE44-BC6A-330EC5790F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="26100" windowHeight="16100" xr2:uid="{2C7B4680-893B-4A42-8DA2-9636C056BE27}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="14660" windowHeight="16100" xr2:uid="{2C7B4680-893B-4A42-8DA2-9636C056BE27}"/>
   </bookViews>
   <sheets>
     <sheet name="Turbines" sheetId="1" r:id="rId1"/>
@@ -594,7 +594,7 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1348,7 +1348,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>